<commit_message>
Initial commit of working system.
</commit_message>
<xml_diff>
--- a/hear/sqlpad/cache/Dq1RSaZyPWG1gGwC.xlsx
+++ b/hear/sqlpad/cache/Dq1RSaZyPWG1gGwC.xlsx
@@ -387,13 +387,13 @@
     </row>
     <row r="2">
       <c r="A2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
         <v>edit</v>
       </c>
       <c r="C2" t="str">
-        <v>1521</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="3">
@@ -401,21 +401,21 @@
         <v>0</v>
       </c>
       <c r="B3" t="str">
-        <v>categorize</v>
+        <v>edit</v>
       </c>
       <c r="C3" t="str">
-        <v>682</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="str">
-        <v>edit</v>
+        <v>categorize</v>
       </c>
       <c r="C4" t="str">
-        <v>610</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="5">
@@ -426,7 +426,7 @@
         <v>categorize</v>
       </c>
       <c r="C5" t="str">
-        <v>488</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="6">
@@ -437,7 +437,7 @@
         <v>new</v>
       </c>
       <c r="C6" t="str">
-        <v>306</v>
+        <v>714</v>
       </c>
     </row>
     <row r="7">
@@ -448,7 +448,7 @@
         <v>log</v>
       </c>
       <c r="C7" t="str">
-        <v>88</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8">
@@ -459,7 +459,7 @@
         <v>log</v>
       </c>
       <c r="C8" t="str">
-        <v>62</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9">
@@ -470,7 +470,7 @@
         <v>new</v>
       </c>
       <c r="C9" t="str">
-        <v>43</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>